<commit_message>
fixed code, added test files
</commit_message>
<xml_diff>
--- a/FinalTest_merged_E0-5_E0-20.xlsx
+++ b/FinalTest_merged_E0-5_E0-20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd192a4dbd6ed64f/University/2018-2019/Final year project/Project/HomeHelpService/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\OneDrive\University\2018-2019\Final year project\Project\HomeHelpService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{09E366D2-A9EE-49D6-8BE7-F7E9133E09B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{30179BAE-7FBA-474D-9117-B4358A1689E1}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{09E366D2-A9EE-49D6-8BE7-F7E9133E09B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{1AE9A4DE-DA59-4BDE-A92B-FA0D197CF1FB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{FC64394E-71EE-4661-8BC1-9AF1B1846853}"/>
+    <workbookView xWindow="3120" yWindow="1845" windowWidth="11925" windowHeight="11655" xr2:uid="{FC64394E-71EE-4661-8BC1-9AF1B1846853}"/>
   </bookViews>
   <sheets>
     <sheet name="E1_UpTo20" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="E3_UpTo20" sheetId="3" r:id="rId3"/>
     <sheet name="E4_UpTo20" sheetId="4" r:id="rId4"/>
     <sheet name="E5_UpTo20" sheetId="5" r:id="rId5"/>
+    <sheet name="E6_UpTo20" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="390">
   <si>
     <t>First Try</t>
   </si>
@@ -1160,6 +1161,51 @@
   </si>
   <si>
     <t>CONSTRAINTS</t>
+  </si>
+  <si>
+    <t>[[17, 6, 5], [16, 3, 9, 10], [15, 8], [14, 7, 11], [13, 2], [12, 0, 4, 1]]</t>
+  </si>
+  <si>
+    <t>[[16, 3, 1], [15, 6, 5, 2], [14, 8], [13, 4], [12, 7, 0], [11, 10, 9]]</t>
+  </si>
+  <si>
+    <t>[[19, 11, 7], [18, 2, 13, 6], [17, 0, 10], [16, 1, 5, 12], [15, 4, 9], [14, 3, 8]]</t>
+  </si>
+  <si>
+    <t>[[25, 0, 12], [24, 3, 13, 15, 19], [23, 1, 10, 11, 14], [22, 8, 4, 9, 6], [21, 16, 7, 5], [20, 17, 2, 18]]</t>
+  </si>
+  <si>
+    <t>[[13, 5], [11, 4], [9, 2, 1], [7, 8], [6, 10], [3, 12, 0]]</t>
+  </si>
+  <si>
+    <t>[[22, 2], [21, 8, 16], [20, 4, 9, 11, 3], [19, 0, 14, 1], [18, 6, 13, 10, 7], [17, 5, 15, 12]]</t>
+  </si>
+  <si>
+    <t>[[16, 3], [15, 8], [14, 6, 2], [13, 10, 9, 0], [12, 4, 1, 5], [11, 7]]</t>
+  </si>
+  <si>
+    <t>[[12, 0], [11, 1], [10, 2], [9, 3], [8, 4], [7, 6, 5]]</t>
+  </si>
+  <si>
+    <t>[[21, 10, 15, 14], [20, 3], [19, 2, 5, 8, 4], [18, 6, 9], [17, 1, 12, 7, 0], [16, 13, 11]]</t>
+  </si>
+  <si>
+    <t>[[11, 3], [10, 1], [9, 2], [8, 0], [7, 5], [6, 4]]</t>
+  </si>
+  <si>
+    <t>[[23, 13, 2, 14], [22, 4, 11, 8, 15], [21, 16, 1, 9], [20, 5, 3, 0, 12], [19, 17, 6, 7], [18, 10]]</t>
+  </si>
+  <si>
+    <t>[[13, 2], [12, 0, 5], [11, 3], [10, 4, 1], [9, 6], [8, 7]]</t>
+  </si>
+  <si>
+    <t>[[20, 1, 12, 0], [19, 3, 11, 5], [18, 6, 13], [17, 10, 14, 8], [16, 4], [15, 2, 9, 7]]</t>
+  </si>
+  <si>
+    <t>[[15, 0], [14, 1], [13, 2], [12, 3], [11, 6, 9, 4], [10, 7, 8, 5]]</t>
+  </si>
+  <si>
+    <t>SUCCESS %</t>
   </si>
 </sst>
 </file>
@@ -1603,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E1EA75-4678-4424-A894-55290945A33A}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,6 +1926,13 @@
       <c r="G10">
         <v>3</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I10" s="9">
+        <f>((COUNTIF(E:E, "First Try") + COUNTIF(E:E, "First Relaxation"))*100)/87</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3450,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D56D6FC-DEB8-49D0-A920-80ABD1483B06}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3728,6 +3781,13 @@
       <c r="G10">
         <v>3</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I10" s="9">
+        <f>((COUNTIF(E:E, "First Try") + COUNTIF(E:E, "First Relaxation"))*100)/100</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -5558,8 +5618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC63CAFF-EF5F-4BC8-8238-D07187688D03}">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5836,6 +5896,13 @@
       <c r="G10">
         <v>4</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I10" s="9">
+        <f>((COUNTIF(E:E, "First Try") + COUNTIF(E:E, "First Relaxation"))*100)/105</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -7767,7 +7834,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8044,6 +8111,13 @@
       <c r="G10">
         <v>5</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I10" s="9">
+        <f>((COUNTIF(E:E, "First Try") + COUNTIF(E:E, "First Relaxation"))*100)/99</f>
+        <v>56.565656565656568</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -9855,7 +9929,7 @@
   <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10132,6 +10206,13 @@
       <c r="G10">
         <v>6</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I10" s="9">
+        <f>((COUNTIF(E:E, "First Try") + COUNTIF(E:E, "First Relaxation"))*100)/109</f>
+        <v>44.036697247706421</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -12136,4 +12217,502 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A9411-6E58-4A5A-8948-841C5554796C}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>0.116980791091918</v>
+      </c>
+      <c r="C2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0.13798022270202601</v>
+      </c>
+      <c r="C3" t="s">
+        <v>382</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="I3" s="7">
+        <f>COUNTIF(E2:E1000, "Error")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.20896744728088301</v>
+      </c>
+      <c r="C4" t="s">
+        <v>379</v>
+      </c>
+      <c r="E4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9.9996566772460896E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0.330947875976562</v>
+      </c>
+      <c r="C6" t="s">
+        <v>388</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="I6" s="9">
+        <f>AVERAGE(B$2:B$1048576)</f>
+        <v>14.07091473278245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>5.3880097866058296</v>
+      </c>
+      <c r="C7" t="s">
+        <v>376</v>
+      </c>
+      <c r="E7">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="I7" s="9">
+        <f>SUM(B$2:B$1048576)</f>
+        <v>267.34737992286654</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>4.5117039680480904</v>
+      </c>
+      <c r="C8" t="s">
+        <v>376</v>
+      </c>
+      <c r="E8">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="I8" s="9">
+        <f>SUM(B$2:B$1048576)/60</f>
+        <v>4.4557896653811087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.181058645248413</v>
+      </c>
+      <c r="C9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>11</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="I9" s="9">
+        <f>MAX(B$2:B$1048576)</f>
+        <v>67.052122831344604</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4.7993888854980398</v>
+      </c>
+      <c r="C10" t="s">
+        <v>376</v>
+      </c>
+      <c r="E10">
+        <v>51</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="I10" s="9">
+        <f>((COUNTIF(E:E, "First Try") + COUNTIF(E:E, "First Relaxation"))*100)/19</f>
+        <v>31.578947368421051</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>23.991958856582599</v>
+      </c>
+      <c r="C11" t="s">
+        <v>375</v>
+      </c>
+      <c r="E11">
+        <v>109</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>18.1979672908782</v>
+      </c>
+      <c r="C12" t="s">
+        <v>375</v>
+      </c>
+      <c r="E12">
+        <v>109</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>24.050690889358499</v>
+      </c>
+      <c r="C13" t="s">
+        <v>377</v>
+      </c>
+      <c r="E13">
+        <v>117</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>5.3874013423919598</v>
+      </c>
+      <c r="C14" t="s">
+        <v>387</v>
+      </c>
+      <c r="E14">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0.92111539840698198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>383</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>62.810128211975098</v>
+      </c>
+      <c r="C16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E16">
+        <v>169</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>67.052122831344604</v>
+      </c>
+      <c r="C17" t="s">
+        <v>380</v>
+      </c>
+      <c r="E17">
+        <v>169</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.58389139175414995</v>
+      </c>
+      <c r="C18" t="s">
+        <v>385</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>26.3116469383239</v>
+      </c>
+      <c r="C19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E19">
+        <v>72</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>22.2654225826263</v>
+      </c>
+      <c r="C20" t="s">
+        <v>378</v>
+      </c>
+      <c r="E20">
+        <v>72</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+    <sortCondition ref="G2:G20"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>